<commit_message>
12.06.2023 All code committed to git hub
</commit_message>
<xml_diff>
--- a/src/main/java/com/amt/testData/QuoteSave.xlsx
+++ b/src/main/java/com/amt/testData/QuoteSave.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t xml:space="preserve">HEJ93780</t>
   </si>
@@ -460,6 +460,54 @@
   </si>
   <si>
     <t>JGO04006</t>
+  </si>
+  <si>
+    <t>JWO64184</t>
+  </si>
+  <si>
+    <t>BBY83031</t>
+  </si>
+  <si>
+    <t>RZP75222</t>
+  </si>
+  <si>
+    <t>KPR35738</t>
+  </si>
+  <si>
+    <t>GRY46566</t>
+  </si>
+  <si>
+    <t>WBB85876</t>
+  </si>
+  <si>
+    <t>NOJ39172</t>
+  </si>
+  <si>
+    <t>OJX15697</t>
+  </si>
+  <si>
+    <t>QHD02977</t>
+  </si>
+  <si>
+    <t>ZOY39884</t>
+  </si>
+  <si>
+    <t>BMI23070</t>
+  </si>
+  <si>
+    <t>DPQ35492</t>
+  </si>
+  <si>
+    <t>THT03416</t>
+  </si>
+  <si>
+    <t>VXJ67664</t>
+  </si>
+  <si>
+    <t>ZHE09143</t>
+  </si>
+  <si>
+    <t>XOR36155</t>
   </si>
 </sst>
 </file>
@@ -569,7 +617,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>111</v>
@@ -639,7 +687,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>57</v>

</xml_diff>